<commit_message>
add new teams new TOs
</commit_message>
<xml_diff>
--- a/esports_teams.xlsx
+++ b/esports_teams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raied\Desktop\eSports_Teams\eSports_Teams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E624451-1F0D-484D-8CCB-5E1DDC4E60F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA385DE5-4AE7-4400-ADF1-16F52109795E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="138">
   <si>
     <t>id</t>
   </si>
@@ -274,6 +274,9 @@
     <t>@DonzEsports</t>
   </si>
   <si>
+    <t>./Avatars/DonzEsports.jpg</t>
+  </si>
+  <si>
     <t>WoLz eSports</t>
   </si>
   <si>
@@ -355,6 +358,9 @@
     <t>@TUWAIQEC</t>
   </si>
   <si>
+    <t>./Avatars/TUWAIQEC.jpg</t>
+  </si>
+  <si>
     <t>Falcon Esports</t>
   </si>
   <si>
@@ -379,6 +385,9 @@
     <t>@WoRzeSports</t>
   </si>
   <si>
+    <t>./Avatars/WoRzeSports.jpg</t>
+  </si>
+  <si>
     <t>Optimistic Force E-Sports</t>
   </si>
   <si>
@@ -415,13 +424,16 @@
     <t>./Avatars/RevSolTeam.jpg</t>
   </si>
   <si>
-    <t>./Avatars/DonzEsports.jpg</t>
-  </si>
-  <si>
-    <t>./Avatars/TUWAIQEC.jpg</t>
-  </si>
-  <si>
-    <t>./Avatars/WoRzeSports.jpg</t>
+    <t>STRONG ESPORTS</t>
+  </si>
+  <si>
+    <t>@STeSports1</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>./Avatars/STeSports1.jpg</t>
   </si>
 </sst>
 </file>
@@ -1281,24 +1293,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1333,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1344,7 +1356,7 @@
         <v>43551</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1367,7 +1379,7 @@
         <v>43549</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1390,7 +1402,7 @@
         <v>43545</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1413,7 +1425,7 @@
         <v>43499</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1436,7 +1448,7 @@
         <v>43520</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1459,7 +1471,7 @@
         <v>43584</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1482,7 +1494,7 @@
         <v>43520</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1505,7 +1517,7 @@
         <v>43510</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1528,7 +1540,7 @@
         <v>43559</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1551,7 +1563,7 @@
         <v>43542</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1574,7 +1586,7 @@
         <v>43586</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1597,7 +1609,7 @@
         <v>43548</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1620,7 +1632,7 @@
         <v>43538</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1643,7 +1655,7 @@
         <v>43529</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1666,7 +1678,7 @@
         <v>43559</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1689,7 +1701,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1712,7 +1724,7 @@
         <v>43492</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1735,7 +1747,7 @@
         <v>43537</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1752,283 +1764,306 @@
         <v>83</v>
       </c>
       <c r="F20" t="s">
-        <v>131</v>
+        <v>84</v>
       </c>
       <c r="G20" s="1">
         <v>43520</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G21" s="1">
         <v>43546</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E22" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F22" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G22" s="1">
         <v>43545</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G23" s="1">
         <v>43545</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F24" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G24" s="1">
         <v>43542</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D25" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E25" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F25" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G25" s="1">
         <v>43516</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D26" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E26" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G26" s="1">
         <v>43499</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E27" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F27" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="G27" s="1">
         <v>43509</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D28" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E28" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F28" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G28" s="1">
         <v>43569</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D29" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E29" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F29" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="G29" s="1">
         <v>43546</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E30" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F30" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G30" s="1">
         <v>43634</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C31" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D31" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E31" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F31" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G31" s="1">
         <v>43636</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C32" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D32" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E32" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F32" t="s">
-        <v>130</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" t="s">
+        <v>135</v>
+      </c>
+      <c r="F33" t="s">
+        <v>137</v>
+      </c>
+      <c r="G33" s="1">
+        <v>43643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>